<commit_message>
clean up labels in raw data
</commit_message>
<xml_diff>
--- a/data-raw/rohdaten.xlsx
+++ b/data-raw/rohdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="96">
   <si>
     <t>id</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>Der Erwerb und die Instandhaltung/Betrieb eines Autos sind für mich zu kostenintensiv</t>
+  </si>
+  <si>
+    <t>kurzname</t>
+  </si>
+  <si>
+    <t>langname</t>
+  </si>
+  <si>
+    <t>Sonstige Anmerkungen</t>
   </si>
 </sst>
 </file>
@@ -622,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
@@ -1544,265 +1553,276 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>50</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add all data to raw file
</commit_message>
<xml_diff>
--- a/data-raw/rohdaten.xlsx
+++ b/data-raw/rohdaten.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="123">
   <si>
     <t>id</t>
   </si>
@@ -316,6 +316,87 @@
   </si>
   <si>
     <t>Sonstige Anmerkungen</t>
+  </si>
+  <si>
+    <t>Ich habe Angst vorm Autofahren</t>
+  </si>
+  <si>
+    <t>45 u. älter</t>
+  </si>
+  <si>
+    <t>Ich habe keine Lust Auto zu fahren</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Aussage zu Gründen, warum keinen Führerschein hat widerspricht sich</t>
+  </si>
+  <si>
+    <t>Habe bis vor zwei Jahren in Wien gelebt und da brauchte ich keinen Führerschein weil ich die Öffentlichen Verkehrsmittel vor der Türe hatte und ich auch wesentlich schneller war doch jetzt brauche ich einen denn in Hartberg sieht das etwas anders aus.</t>
+  </si>
+  <si>
+    <t>In Wien keinen gebraucht, in Hartberg jetzt schon</t>
+  </si>
+  <si>
+    <t>Ich bin derzeit zu beschäftigt bzw. habe zu wenig Zeit, um einen Führerschein zu machen</t>
+  </si>
+  <si>
+    <t>Ich bevorzuge es zu Fuß zu gehen</t>
+  </si>
+  <si>
+    <t>Berufsbildende Schule</t>
+  </si>
+  <si>
+    <t>Derzeit ohne feste Anstellung / arbeitssuchend</t>
+  </si>
+  <si>
+    <t>Frage 7 nur angekreuzt, daher keine Daten eingegeben.</t>
+  </si>
+  <si>
+    <t>Reihung von 7 widerspricht 6: Fälschung?</t>
+  </si>
+  <si>
+    <t>35-39</t>
+  </si>
+  <si>
+    <t>Mehrfache Angabe bei 6, nicht kongruent mit 7; daher keine Dateneingabe</t>
+  </si>
+  <si>
+    <t>Fragebogen offenbar ab Frage 8 abgebrochen.</t>
+  </si>
+  <si>
+    <t>40-44</t>
+  </si>
+  <si>
+    <t>Invalidität, gesundheitliche Probleme, Sehschwäche</t>
+  </si>
+  <si>
+    <t>Pensioniert</t>
+  </si>
+  <si>
+    <t>Ich halte die negativen Umweltfolgen des Autofahrens für zu gravierend</t>
+  </si>
+  <si>
+    <t>Ich komme aus eine große Stadt wo mann keine Auto braucht weil der Bus und U-Bahn sehr efizient sind</t>
+  </si>
+  <si>
+    <t>Auto in großer Stadt nicht notwendig</t>
+  </si>
+  <si>
+    <t>zu jung</t>
+  </si>
+  <si>
+    <t>Verbauung der Umwelt</t>
+  </si>
+  <si>
+    <t>Autounfall</t>
+  </si>
+  <si>
+    <t>In Graz ist der Besitz eines Autos nicht notwendig</t>
+  </si>
+  <si>
+    <t>Fragen 6 und 7 falsch ausgefülllt; keine Dateneingabe</t>
   </si>
 </sst>
 </file>
@@ -629,10 +710,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AF101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF14" sqref="AF14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1435,115 +1517,3879 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC15">
+        <v>10</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>5</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC16">
+        <v>2.5</v>
+      </c>
+      <c r="AD16">
+        <v>2</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>90</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC17">
+        <v>2</v>
+      </c>
+      <c r="AD17">
+        <v>4</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>2</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC18">
+        <v>5</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>2</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>98</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC22">
+        <v>0.5</v>
+      </c>
+      <c r="AD22">
+        <v>1</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>2</v>
+      </c>
+      <c r="T23">
+        <v>3</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC23">
+        <v>8</v>
+      </c>
+      <c r="AD23">
+        <v>2.5</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>1.5</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P25">
+        <v>2</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0.75</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="T26">
+        <v>3</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>1</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC27">
+        <v>1.5</v>
+      </c>
+      <c r="AD27">
+        <v>1</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC28">
+        <v>0.5</v>
+      </c>
+      <c r="AD28">
+        <v>6</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>3</v>
+      </c>
+      <c r="Q29">
+        <v>5</v>
+      </c>
+      <c r="R29">
+        <v>4</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC29">
+        <v>4</v>
+      </c>
+      <c r="AD29">
+        <v>10</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>104</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC30">
+        <v>6</v>
+      </c>
+      <c r="AD30">
+        <v>6</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>98</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+      <c r="T31">
+        <v>3</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>7</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>90</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="O32">
+        <v>3</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>4</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC33">
+        <v>2</v>
+      </c>
+      <c r="AD33">
+        <v>2</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC34">
+        <v>2.5</v>
+      </c>
+      <c r="AD34">
+        <v>2.5</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35">
+        <v>11</v>
+      </c>
+      <c r="K35">
+        <v>6</v>
+      </c>
+      <c r="L35">
+        <v>4</v>
+      </c>
+      <c r="M35">
+        <v>7</v>
+      </c>
+      <c r="N35">
+        <v>12</v>
+      </c>
+      <c r="O35">
+        <v>8</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>9</v>
+      </c>
+      <c r="R35">
+        <v>5</v>
+      </c>
+      <c r="S35">
+        <v>2</v>
+      </c>
+      <c r="T35">
+        <v>3</v>
+      </c>
+      <c r="U35">
+        <v>10</v>
+      </c>
+      <c r="V35">
+        <v>13</v>
+      </c>
+      <c r="W35">
+        <v>14</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC35">
+        <v>0.5</v>
+      </c>
+      <c r="AD35">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" t="s">
+        <v>90</v>
+      </c>
+      <c r="M36">
+        <v>3</v>
+      </c>
+      <c r="O36">
+        <v>2</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC36">
+        <v>2</v>
+      </c>
+      <c r="AD36">
+        <v>2</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>18</v>
+      </c>
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" t="s">
+        <v>90</v>
+      </c>
+      <c r="J37">
+        <v>7</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <v>5</v>
+      </c>
+      <c r="Q37">
+        <v>6</v>
+      </c>
+      <c r="R37">
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <v>3</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>8</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC37">
+        <v>4.5</v>
+      </c>
+      <c r="AD37">
+        <v>4.5</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
+        <v>92</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>3</v>
+      </c>
+      <c r="S38">
+        <v>2</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC38">
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <v>4</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39">
+        <v>18</v>
+      </c>
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q39">
+        <v>2</v>
+      </c>
+      <c r="R39">
+        <v>3</v>
+      </c>
+      <c r="T39">
+        <v>4</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC39">
+        <v>0</v>
+      </c>
+      <c r="AD39">
+        <v>3</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" t="s">
+        <v>58</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC40">
+        <v>1</v>
+      </c>
+      <c r="AD40">
+        <v>2</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" t="s">
+        <v>92</v>
+      </c>
+      <c r="K41">
+        <v>3</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>4</v>
+      </c>
+      <c r="S41">
+        <v>2</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC41">
+        <v>0</v>
+      </c>
+      <c r="AD41">
+        <v>4</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>32</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>2</v>
+      </c>
+      <c r="R42">
+        <v>3</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC42">
+        <v>0</v>
+      </c>
+      <c r="AD42">
+        <v>2</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC43">
+        <v>0</v>
+      </c>
+      <c r="AD43">
+        <v>3</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>32</v>
+      </c>
+      <c r="L44">
+        <v>3</v>
+      </c>
+      <c r="M44">
+        <v>4</v>
+      </c>
+      <c r="N44">
+        <v>5</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>6</v>
+      </c>
+      <c r="R44">
+        <v>8</v>
+      </c>
+      <c r="S44">
+        <v>7</v>
+      </c>
+      <c r="T44">
+        <v>2</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC44">
+        <v>2</v>
+      </c>
+      <c r="AD44">
+        <v>1</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" t="s">
+        <v>38</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>6</v>
+      </c>
+      <c r="M45">
+        <v>7</v>
+      </c>
+      <c r="O45">
+        <v>2</v>
+      </c>
+      <c r="Q45">
+        <v>3</v>
+      </c>
+      <c r="S45">
+        <v>4</v>
+      </c>
+      <c r="T45">
+        <v>5</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC45">
+        <v>0</v>
+      </c>
+      <c r="AD45">
+        <v>2</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
+        <v>90</v>
+      </c>
+      <c r="J46">
+        <v>3</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+      <c r="N46">
+        <v>6</v>
+      </c>
+      <c r="O46">
+        <v>4</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46">
+        <v>5</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC46">
+        <v>0</v>
+      </c>
+      <c r="AD46">
+        <v>1</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC47">
+        <v>0</v>
+      </c>
+      <c r="AD47">
+        <v>1</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" t="s">
+        <v>90</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+      <c r="Q48">
+        <v>3</v>
+      </c>
+      <c r="S48">
+        <v>2</v>
+      </c>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC48">
+        <v>3</v>
+      </c>
+      <c r="AD48">
+        <v>1</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" t="s">
+        <v>90</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
+      </c>
+      <c r="K49">
+        <v>2</v>
+      </c>
+      <c r="P49">
+        <v>3</v>
+      </c>
+      <c r="Q49">
+        <v>5</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <v>4</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC49">
+        <v>1</v>
+      </c>
+      <c r="AD49">
+        <v>4</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" t="s">
+        <v>58</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+      <c r="R50">
+        <v>6</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>3</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" t="s">
+        <v>96</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC51">
+        <v>3.5</v>
+      </c>
+      <c r="AD51">
+        <v>1</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52">
+        <v>19</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+      <c r="F52" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" t="s">
+        <v>103</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="U52">
+        <v>1</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC52">
+        <v>6</v>
+      </c>
+      <c r="AD52">
+        <v>2</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53">
+        <v>19</v>
+      </c>
+      <c r="E53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" t="s">
+        <v>104</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <v>3</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC53">
+        <v>0.5</v>
+      </c>
+      <c r="AD53">
+        <v>0.5</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" t="s">
+        <v>32</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC54">
+        <v>0.5</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" t="s">
+        <v>112</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" t="s">
+        <v>113</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="V55">
+        <v>1</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC55">
+        <v>0</v>
+      </c>
+      <c r="AD55">
+        <v>6</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>92</v>
+      </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+      <c r="R56">
+        <v>3</v>
+      </c>
+      <c r="S56">
+        <v>2</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC56">
+        <v>3</v>
+      </c>
+      <c r="AD56">
+        <v>0.5</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" t="s">
+        <v>37</v>
+      </c>
+      <c r="F57" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" t="s">
+        <v>96</v>
+      </c>
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>3</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC57">
+        <v>0</v>
+      </c>
+      <c r="AD57">
+        <v>0</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58" t="s">
+        <v>37</v>
+      </c>
+      <c r="F58" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" t="s">
+        <v>90</v>
+      </c>
+      <c r="L58">
+        <v>4</v>
+      </c>
+      <c r="O58">
+        <v>5</v>
+      </c>
+      <c r="Q58">
+        <v>6</v>
+      </c>
+      <c r="R58">
+        <v>2</v>
+      </c>
+      <c r="S58">
+        <v>3</v>
+      </c>
+      <c r="T58">
+        <v>1</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC58">
+        <v>8</v>
+      </c>
+      <c r="AD58">
+        <v>2</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59">
+        <v>19</v>
+      </c>
+      <c r="E59" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" t="s">
+        <v>115</v>
+      </c>
+      <c r="K59">
+        <v>3</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>2</v>
+      </c>
+      <c r="Q59">
+        <v>5</v>
+      </c>
+      <c r="R59">
+        <v>4</v>
+      </c>
+      <c r="S59">
+        <v>6</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC59">
+        <v>3</v>
+      </c>
+      <c r="AD59">
+        <v>3</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" t="s">
+        <v>37</v>
+      </c>
+      <c r="F60" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" t="s">
+        <v>38</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+      <c r="Q60">
+        <v>3</v>
+      </c>
+      <c r="R60">
+        <v>4</v>
+      </c>
+      <c r="S60">
+        <v>5</v>
+      </c>
+      <c r="T60">
+        <v>6</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC60">
+        <v>5</v>
+      </c>
+      <c r="AD60">
+        <v>1</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" t="s">
+        <v>109</v>
+      </c>
+      <c r="E61" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" t="s">
+        <v>45</v>
+      </c>
+      <c r="H61" t="s">
+        <v>116</v>
+      </c>
+      <c r="P61">
+        <v>2</v>
+      </c>
+      <c r="X61">
+        <v>1</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC61">
+        <v>6</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62">
+        <v>18</v>
+      </c>
+      <c r="E62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" t="s">
+        <v>38</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>3</v>
+      </c>
+      <c r="R62">
+        <v>5</v>
+      </c>
+      <c r="S62">
+        <v>4</v>
+      </c>
+      <c r="T62">
+        <v>2</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC62">
+        <v>1</v>
+      </c>
+      <c r="AD62">
+        <v>4</v>
+      </c>
+      <c r="AE62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" t="s">
+        <v>54</v>
+      </c>
+      <c r="E63" t="s">
+        <v>37</v>
+      </c>
+      <c r="F63" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" t="s">
+        <v>98</v>
+      </c>
+      <c r="N63">
+        <v>2</v>
+      </c>
+      <c r="O63">
+        <v>1</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC63">
+        <v>0</v>
+      </c>
+      <c r="AD63">
+        <v>9</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" t="s">
+        <v>109</v>
+      </c>
+      <c r="E64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" t="s">
+        <v>90</v>
+      </c>
+      <c r="L64">
+        <v>2</v>
+      </c>
+      <c r="T64">
+        <v>1</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC64">
+        <v>8</v>
+      </c>
+      <c r="AD64">
+        <v>1</v>
+      </c>
+      <c r="AE64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" t="s">
+        <v>37</v>
+      </c>
+      <c r="F65" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65" t="s">
+        <v>38</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="T65">
+        <v>2</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC65">
+        <v>0</v>
+      </c>
+      <c r="AD65">
+        <v>3</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66">
+        <v>17</v>
+      </c>
+      <c r="E66" t="s">
+        <v>37</v>
+      </c>
+      <c r="F66" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" t="s">
+        <v>45</v>
+      </c>
+      <c r="H66" t="s">
+        <v>118</v>
+      </c>
+      <c r="K66">
+        <v>2</v>
+      </c>
+      <c r="X66">
+        <v>1</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC66">
+        <v>2</v>
+      </c>
+      <c r="AD66">
+        <v>4</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" t="s">
+        <v>31</v>
+      </c>
+      <c r="F67" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" t="s">
+        <v>90</v>
+      </c>
+      <c r="L67">
+        <v>2</v>
+      </c>
+      <c r="T67">
+        <v>1</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC67">
+        <v>0</v>
+      </c>
+      <c r="AD67">
+        <v>2</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" t="s">
+        <v>54</v>
+      </c>
+      <c r="E68" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G68" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q68">
+        <v>3</v>
+      </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
+      <c r="T68">
+        <v>2</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC68">
+        <v>0.5</v>
+      </c>
+      <c r="AD68">
+        <v>1</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69">
+        <v>19</v>
+      </c>
+      <c r="E69" t="s">
+        <v>31</v>
+      </c>
+      <c r="F69" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" t="s">
+        <v>98</v>
+      </c>
+      <c r="O69">
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>2</v>
+      </c>
+      <c r="R69">
+        <v>3</v>
+      </c>
+      <c r="S69">
+        <v>5</v>
+      </c>
+      <c r="T69">
+        <v>4</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC69">
+        <v>2</v>
+      </c>
+      <c r="AD69">
+        <v>3</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" t="s">
+        <v>36</v>
+      </c>
+      <c r="E70" t="s">
+        <v>31</v>
+      </c>
+      <c r="F70" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" t="s">
+        <v>38</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>7</v>
+      </c>
+      <c r="O70">
+        <v>2</v>
+      </c>
+      <c r="Q70">
+        <v>6</v>
+      </c>
+      <c r="R70">
+        <v>4</v>
+      </c>
+      <c r="S70">
+        <v>3</v>
+      </c>
+      <c r="T70">
+        <v>5</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC70">
+        <v>1</v>
+      </c>
+      <c r="AD70">
+        <v>1</v>
+      </c>
+      <c r="AE70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" t="s">
+        <v>31</v>
+      </c>
+      <c r="F71" t="s">
+        <v>30</v>
+      </c>
+      <c r="G71" t="s">
+        <v>90</v>
+      </c>
+      <c r="K71">
+        <v>7</v>
+      </c>
+      <c r="L71">
+        <v>6</v>
+      </c>
+      <c r="O71">
+        <v>5</v>
+      </c>
+      <c r="Q71">
+        <v>8</v>
+      </c>
+      <c r="R71">
+        <v>3</v>
+      </c>
+      <c r="S71">
+        <v>2</v>
+      </c>
+      <c r="T71">
+        <v>1</v>
+      </c>
+      <c r="U71">
+        <v>4</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC71">
+        <v>1</v>
+      </c>
+      <c r="AD71">
+        <v>4</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72">
+        <v>19</v>
+      </c>
+      <c r="E72" t="s">
+        <v>37</v>
+      </c>
+      <c r="F72" t="s">
+        <v>30</v>
+      </c>
+      <c r="G72" t="s">
+        <v>58</v>
+      </c>
+      <c r="K72">
+        <v>8</v>
+      </c>
+      <c r="L72">
+        <v>5</v>
+      </c>
+      <c r="O72">
+        <v>7</v>
+      </c>
+      <c r="Q72">
+        <v>6</v>
+      </c>
+      <c r="R72">
+        <v>2</v>
+      </c>
+      <c r="S72">
+        <v>1</v>
+      </c>
+      <c r="T72">
+        <v>3</v>
+      </c>
+      <c r="U72">
+        <v>4</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC72">
+        <v>3</v>
+      </c>
+      <c r="AD72">
+        <v>3</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>30</v>
+      </c>
+      <c r="C73" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" t="s">
+        <v>31</v>
+      </c>
+      <c r="F73" t="s">
+        <v>30</v>
+      </c>
+      <c r="G73" t="s">
+        <v>115</v>
+      </c>
+      <c r="J73">
+        <v>9</v>
+      </c>
+      <c r="K73">
+        <v>8</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73">
+        <v>4</v>
+      </c>
+      <c r="N73">
+        <v>10</v>
+      </c>
+      <c r="O73">
+        <v>11</v>
+      </c>
+      <c r="P73">
+        <v>12</v>
+      </c>
+      <c r="Q73">
+        <v>3</v>
+      </c>
+      <c r="R73">
+        <v>6</v>
+      </c>
+      <c r="S73">
+        <v>5</v>
+      </c>
+      <c r="T73">
+        <v>2</v>
+      </c>
+      <c r="U73">
+        <v>7</v>
+      </c>
+      <c r="V73">
+        <v>13</v>
+      </c>
+      <c r="W73">
+        <v>14</v>
+      </c>
+      <c r="X73">
+        <v>15</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC73">
+        <v>3.5</v>
+      </c>
+      <c r="AD73">
+        <v>1</v>
+      </c>
+      <c r="AE73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" t="s">
+        <v>54</v>
+      </c>
+      <c r="E74" t="s">
+        <v>31</v>
+      </c>
+      <c r="F74" t="s">
+        <v>47</v>
+      </c>
+      <c r="G74" t="s">
+        <v>80</v>
+      </c>
+      <c r="K74">
+        <v>2</v>
+      </c>
+      <c r="N74">
+        <v>3</v>
+      </c>
+      <c r="U74">
+        <v>4</v>
+      </c>
+      <c r="W74">
+        <v>1</v>
+      </c>
+      <c r="X74">
+        <v>5</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC74">
+        <v>2</v>
+      </c>
+      <c r="AD74">
+        <v>2</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" t="s">
+        <v>36</v>
+      </c>
+      <c r="E75" t="s">
+        <v>37</v>
+      </c>
+      <c r="F75" t="s">
+        <v>30</v>
+      </c>
+      <c r="G75" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC75">
+        <v>1</v>
+      </c>
+      <c r="AD75">
+        <v>4</v>
+      </c>
+      <c r="AE75" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF75" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>30</v>
+      </c>
+      <c r="C76" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E76" t="s">
+        <v>31</v>
+      </c>
+      <c r="F76" t="s">
+        <v>30</v>
+      </c>
+      <c r="G76" t="s">
+        <v>90</v>
+      </c>
+      <c r="K76">
+        <v>2</v>
+      </c>
+      <c r="L76">
+        <v>4</v>
+      </c>
+      <c r="Q76">
+        <v>3</v>
+      </c>
+      <c r="R76">
+        <v>6</v>
+      </c>
+      <c r="S76">
+        <v>5</v>
+      </c>
+      <c r="T76">
+        <v>1</v>
+      </c>
+      <c r="X76">
+        <v>7</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA76" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC76">
+        <v>0</v>
+      </c>
+      <c r="AD76">
+        <v>2</v>
+      </c>
+      <c r="AE76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" t="s">
+        <v>36</v>
+      </c>
+      <c r="E77" t="s">
+        <v>31</v>
+      </c>
+      <c r="F77" t="s">
+        <v>30</v>
+      </c>
+      <c r="G77" t="s">
+        <v>90</v>
+      </c>
+      <c r="K77">
+        <v>2</v>
+      </c>
+      <c r="R77">
+        <v>3</v>
+      </c>
+      <c r="T77">
+        <v>1</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC77">
+        <v>1</v>
+      </c>
+      <c r="AD77">
+        <v>2</v>
+      </c>
+      <c r="AE77" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C78" t="s">
+        <v>30</v>
+      </c>
+      <c r="D78" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78" t="s">
+        <v>37</v>
+      </c>
+      <c r="F78" t="s">
+        <v>30</v>
+      </c>
+      <c r="G78" t="s">
+        <v>32</v>
+      </c>
+      <c r="P78">
+        <v>1</v>
+      </c>
+      <c r="T78">
+        <v>2</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA78" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC78">
+        <v>4</v>
+      </c>
+      <c r="AD78">
+        <v>0</v>
+      </c>
+      <c r="AE78" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" t="s">
+        <v>30</v>
+      </c>
+      <c r="D79" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79" t="s">
+        <v>37</v>
+      </c>
+      <c r="F79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G79" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q79">
+        <v>2</v>
+      </c>
+      <c r="U79">
+        <v>1</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC79">
+        <v>1.5</v>
+      </c>
+      <c r="AD79">
+        <v>2.5</v>
+      </c>
+      <c r="AE79" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" t="s">
+        <v>37</v>
+      </c>
+      <c r="F80" t="s">
+        <v>30</v>
+      </c>
+      <c r="G80" t="s">
+        <v>98</v>
+      </c>
+      <c r="O80">
+        <v>1</v>
+      </c>
+      <c r="R80">
+        <v>3</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC80">
+        <v>5</v>
+      </c>
+      <c r="AD80">
+        <v>0</v>
+      </c>
+      <c r="AE80" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>30</v>
+      </c>
+      <c r="C81" t="s">
+        <v>30</v>
+      </c>
+      <c r="D81" t="s">
+        <v>54</v>
+      </c>
+      <c r="E81" t="s">
+        <v>31</v>
+      </c>
+      <c r="F81" t="s">
+        <v>30</v>
+      </c>
+      <c r="G81" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+      <c r="R81">
+        <v>2</v>
+      </c>
+      <c r="V81">
+        <v>3</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA81" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC81">
+        <v>3.5</v>
+      </c>
+      <c r="AD81">
+        <v>3.5</v>
+      </c>
+      <c r="AE81" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" t="s">
+        <v>30</v>
+      </c>
+      <c r="D82">
+        <v>18</v>
+      </c>
+      <c r="E82" t="s">
+        <v>37</v>
+      </c>
+      <c r="F82" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA82" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC82">
+        <v>4</v>
+      </c>
+      <c r="AD82">
+        <v>3</v>
+      </c>
+      <c r="AE82" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" t="s">
+        <v>30</v>
+      </c>
+      <c r="D83">
+        <v>18</v>
+      </c>
+      <c r="E83" t="s">
+        <v>31</v>
+      </c>
+      <c r="F83" t="s">
+        <v>30</v>
+      </c>
+      <c r="G83" t="s">
+        <v>38</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>4</v>
+      </c>
+      <c r="O83">
+        <v>3</v>
+      </c>
+      <c r="Q83">
+        <v>2</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC83">
+        <v>3</v>
+      </c>
+      <c r="AD83">
+        <v>3</v>
+      </c>
+      <c r="AE83" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>30</v>
+      </c>
+      <c r="C84" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" t="s">
+        <v>36</v>
+      </c>
+      <c r="E84" t="s">
+        <v>37</v>
+      </c>
+      <c r="F84" t="s">
+        <v>30</v>
+      </c>
+      <c r="G84" t="s">
+        <v>98</v>
+      </c>
+      <c r="O84">
+        <v>1</v>
+      </c>
+      <c r="Q84">
+        <v>2</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC84">
+        <v>0</v>
+      </c>
+      <c r="AD84">
+        <v>4</v>
+      </c>
+      <c r="AE84" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" t="s">
+        <v>30</v>
+      </c>
+      <c r="D85">
+        <v>16</v>
+      </c>
+      <c r="E85" t="s">
+        <v>31</v>
+      </c>
+      <c r="F85" t="s">
+        <v>30</v>
+      </c>
+      <c r="G85" t="s">
+        <v>32</v>
+      </c>
+      <c r="I85">
+        <v>2</v>
+      </c>
+      <c r="P85">
+        <v>1</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC85">
+        <v>1</v>
+      </c>
+      <c r="AD85">
+        <v>3</v>
+      </c>
+      <c r="AE85" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86">
+        <v>19</v>
+      </c>
+      <c r="E86" t="s">
+        <v>37</v>
+      </c>
+      <c r="F86" t="s">
+        <v>30</v>
+      </c>
+      <c r="G86" t="s">
+        <v>96</v>
+      </c>
+      <c r="N86">
+        <v>1</v>
+      </c>
+      <c r="Q86">
+        <v>2</v>
+      </c>
+      <c r="R86">
+        <v>3</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC86">
+        <v>5</v>
+      </c>
+      <c r="AD86">
+        <v>1</v>
+      </c>
+      <c r="AE86" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1555,7 +5401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove ids for non-existing ppl
</commit_message>
<xml_diff>
--- a/data-raw/rohdaten.xlsx
+++ b/data-raw/rohdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -710,11 +710,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF101"/>
+  <dimension ref="A1:AF86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5315,81 +5315,6 @@
       </c>
       <c r="AE86" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>